<commit_message>
change RAM to 1.8V and fix BGA clearance for manf
</commit_message>
<xml_diff>
--- a/Project Outputs for PS Digital Test v1.0.0/Digikey BOM-PS Digital Test v1.0.0.xlsx
+++ b/Project Outputs for PS Digital Test v1.0.0/Digikey BOM-PS Digital Test v1.0.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4C1096-213B-41E4-8F56-ADED8162534B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D190D6AD-DC9D-4439-857A-B18E88469932}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="5670" windowWidth="28800" windowHeight="8760" xr2:uid="{252D1A5E-217B-45CF-BE29-EE699E4677DF}"/>
+    <workbookView xWindow="5205" yWindow="5670" windowWidth="28800" windowHeight="8760" xr2:uid="{7EBC7D2E-69CE-4D97-B5C9-BF3629178980}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey BOM-PS Digital Test v1." sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="196">
   <si>
     <t>Comment</t>
   </si>
@@ -58,7 +58,7 @@
     <t>TP</t>
   </si>
   <si>
-    <t>+3.3V, +5V_USB, DONE, FCS, FMISO, FMOSI, FSCK, GND, INTN, JTEN, PGMN, Vref</t>
+    <t>+1.8V, +3.3V, +5V_USB, DONE, FCS, FMISO, FMOSI, FSCK, GND, INTN, JTEN, PGMN, Vref</t>
   </si>
   <si>
     <t>TESTPOINT024</t>
@@ -103,7 +103,7 @@
     <t>10V</t>
   </si>
   <si>
-    <t>C12</t>
+    <t>C12, C31, C32</t>
   </si>
   <si>
     <t>Murata Electronics</t>
@@ -337,16 +337,16 @@
     <t>P9</t>
   </si>
   <si>
-    <t>0.1HDR1X3P</t>
-  </si>
-  <si>
-    <t>22-11-2032</t>
-  </si>
-  <si>
-    <t>Connector, Header, 0.1", 3 Positions, Male, 0.1" Spacing, 4A, 250V, 0.24" Long, 0.125" Tail, 15u" Select Gold, Polarized, Locking Ramp, Vertical</t>
-  </si>
-  <si>
-    <t>WM2701-ND</t>
+    <t>0.1HDR1X4P</t>
+  </si>
+  <si>
+    <t>22-11-2042</t>
+  </si>
+  <si>
+    <t>Connector, Header, 0.1", 4 Positions, Male, 0.1" Spacing, 4A, 250V, 0.24" Long, 0.125" Tail, 15u" Select Gold, Polarized, Locking Ramp, Vert</t>
+  </si>
+  <si>
+    <t>WM2702-ND</t>
   </si>
   <si>
     <t>Bias Power</t>
@@ -596,6 +596,24 @@
   </si>
   <si>
     <t>EMI2121MTTAGOSCT-ND</t>
+  </si>
+  <si>
+    <t>1.8V</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>SOT23-12-3TOP</t>
+  </si>
+  <si>
+    <t>MCP1703T-1802E/CB</t>
+  </si>
+  <si>
+    <t>IC, Voltage Regulator, 1.8Vout, 2.7-16Vin, 200mA, -40°C ~ 125°C, SOT-23, SMD</t>
+  </si>
+  <si>
+    <t>MCP1703T-1802E/CBCT-ND</t>
   </si>
 </sst>
 </file>
@@ -978,8 +996,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39920AB5-3BEB-4D72-8045-AA515B110A1D}">
-  <dimension ref="A1:I30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6050898E-0CD5-4C3F-BE21-2BCC37500487}">
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1037,7 +1055,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>15</v>
@@ -1095,7 +1113,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
@@ -1856,6 +1874,35 @@
       </c>
       <c r="I30" s="2" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>